<commit_message>
removed company and personal info from pass example
</commit_message>
<xml_diff>
--- a/PassRFID.xlsx
+++ b/PassRFID.xlsx
@@ -278,15 +278,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -297,6 +288,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -318,6 +318,44 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>476141</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19222</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="390525" y="304800"/>
+          <a:ext cx="3133616" cy="1981372"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -702,74 +740,6 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 39"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="400050" y="323850"/>
-          <a:ext cx="3133725" cy="1981200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
@@ -1114,123 +1084,123 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B17:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="16384" width="9.140625" style="16"/>
   </cols>
   <sheetData>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="16" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="16" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="16" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="21" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="17" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="2:6" ht="13.5" x14ac:dyDescent="0.2">
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F24" s="21" t="s">
+      <c r="F24" s="18" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="19" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="16" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C32" s="23"/>
-      <c r="D32" s="20" t="s">
+      <c r="C32" s="20"/>
+      <c r="D32" s="17" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="19" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="16" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B36" s="19" t="s">
+      <c r="B36" s="16" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="2:6" ht="14.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="19" t="s">
+      <c r="C38" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E38" s="20">
+      <c r="E38" s="17">
         <f>HEX2DEC(B38)</f>
         <v>1211</v>
       </c>
-      <c r="F38" s="19" t="s">
+      <c r="F38" s="16" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" s="19" t="s">
+      <c r="B40" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="19" t="s">
+      <c r="B41" s="16" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="16" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B44" s="22"/>
+      <c r="B44" s="19"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B45" s="22"/>
+      <c r="B45" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1563,207 +1533,207 @@
       </c>
     </row>
     <row r="6" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="str">
+      <c r="A6" s="22" t="str">
         <f t="shared" ref="A6" si="0">BIN2HEX(A5&amp;B5&amp;C5&amp;D5)</f>
         <v>8</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17" t="str">
+      <c r="B6" s="22"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22" t="str">
         <f t="shared" ref="E6" si="1">BIN2HEX(E5&amp;F5&amp;G5&amp;H5)</f>
         <v>2</v>
       </c>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17" t="str">
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22" t="str">
         <f t="shared" ref="I6" si="2">BIN2HEX(I5&amp;J5&amp;K5&amp;L5)</f>
         <v>0</v>
       </c>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17" t="str">
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22" t="str">
         <f t="shared" ref="M6" si="3">BIN2HEX(M5&amp;N5&amp;O5&amp;P5)</f>
         <v>0</v>
       </c>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17" t="str">
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22" t="str">
         <f t="shared" ref="Q6" si="4">BIN2HEX(Q5&amp;R5&amp;S5&amp;T5)</f>
         <v>0</v>
       </c>
-      <c r="R6" s="17"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17" t="str">
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22" t="str">
         <f t="shared" ref="U6" si="5">BIN2HEX(U5&amp;V5&amp;W5&amp;X5)</f>
         <v>F</v>
       </c>
-      <c r="V6" s="17"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
-      <c r="Y6" s="17" t="str">
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22" t="str">
         <f t="shared" ref="Y6" si="6">BIN2HEX(Y5&amp;Z5&amp;AA5&amp;AB5)</f>
         <v>7</v>
       </c>
-      <c r="Z6" s="17"/>
-      <c r="AA6" s="17"/>
-      <c r="AB6" s="17"/>
-      <c r="AC6" s="17" t="str">
+      <c r="Z6" s="22"/>
+      <c r="AA6" s="22"/>
+      <c r="AB6" s="22"/>
+      <c r="AC6" s="22" t="str">
         <f t="shared" ref="AC6" si="7">BIN2HEX(AC5&amp;AD5&amp;AE5&amp;AF5)</f>
         <v>F</v>
       </c>
-      <c r="AD6" s="17"/>
-      <c r="AE6" s="17"/>
-      <c r="AF6" s="17"/>
-      <c r="AG6" s="17" t="str">
+      <c r="AD6" s="22"/>
+      <c r="AE6" s="22"/>
+      <c r="AF6" s="22"/>
+      <c r="AG6" s="22" t="str">
         <f t="shared" ref="AG6" si="8">BIN2HEX(AG5&amp;AH5&amp;AI5&amp;AJ5)</f>
         <v>4</v>
       </c>
-      <c r="AH6" s="17"/>
-      <c r="AI6" s="17"/>
-      <c r="AJ6" s="17"/>
-      <c r="AK6" s="16" t="str">
+      <c r="AH6" s="22"/>
+      <c r="AI6" s="22"/>
+      <c r="AJ6" s="22"/>
+      <c r="AK6" s="21" t="str">
         <f t="shared" ref="AK6" si="9">BIN2HEX(AK5&amp;AL5&amp;AM5&amp;AN5)</f>
         <v>D</v>
       </c>
-      <c r="AL6" s="16"/>
-      <c r="AM6" s="16"/>
-      <c r="AN6" s="16"/>
-      <c r="AO6" s="16" t="str">
+      <c r="AL6" s="21"/>
+      <c r="AM6" s="21"/>
+      <c r="AN6" s="21"/>
+      <c r="AO6" s="21" t="str">
         <f t="shared" ref="AO6" si="10">BIN2HEX(AO5&amp;AP5&amp;AQ5&amp;AR5)</f>
         <v>B</v>
       </c>
-      <c r="AP6" s="16"/>
-      <c r="AQ6" s="16"/>
-      <c r="AR6" s="16"/>
-      <c r="AS6" s="16" t="str">
+      <c r="AP6" s="21"/>
+      <c r="AQ6" s="21"/>
+      <c r="AR6" s="21"/>
+      <c r="AS6" s="21" t="str">
         <f t="shared" ref="AS6" si="11">BIN2HEX(AS5&amp;AT5&amp;AU5&amp;AV5)</f>
         <v>B</v>
       </c>
-      <c r="AT6" s="16"/>
-      <c r="AU6" s="16"/>
-      <c r="AV6" s="16"/>
-      <c r="AW6" s="16" t="str">
+      <c r="AT6" s="21"/>
+      <c r="AU6" s="21"/>
+      <c r="AV6" s="21"/>
+      <c r="AW6" s="21" t="str">
         <f t="shared" ref="AW6" si="12">BIN2HEX(AW5&amp;AX5&amp;AY5&amp;AZ5)</f>
         <v>8</v>
       </c>
-      <c r="AX6" s="16"/>
-      <c r="AY6" s="16"/>
-      <c r="AZ6" s="16"/>
-      <c r="BA6" s="16" t="str">
+      <c r="AX6" s="21"/>
+      <c r="AY6" s="21"/>
+      <c r="AZ6" s="21"/>
+      <c r="BA6" s="21" t="str">
         <f>BIN2HEX(BA5&amp;BB5&amp;BC5&amp;BD5)</f>
         <v>6</v>
       </c>
-      <c r="BB6" s="16"/>
-      <c r="BC6" s="16"/>
-      <c r="BD6" s="16"/>
+      <c r="BB6" s="21"/>
+      <c r="BC6" s="21"/>
+      <c r="BD6" s="21"/>
       <c r="BE6" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="22">
         <f t="shared" ref="A7" si="13">HEX2DEC(A6)</f>
         <v>8</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22">
         <f t="shared" ref="E7" si="14">HEX2DEC(E6)</f>
         <v>2</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17">
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="22"/>
+      <c r="I7" s="22">
         <f t="shared" ref="I7" si="15">HEX2DEC(I6)</f>
         <v>0</v>
       </c>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17">
+      <c r="J7" s="22"/>
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="22">
         <f t="shared" ref="M7" si="16">HEX2DEC(M6)</f>
         <v>0</v>
       </c>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17">
+      <c r="N7" s="22"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22">
         <f t="shared" ref="Q7" si="17">HEX2DEC(Q6)</f>
         <v>0</v>
       </c>
-      <c r="R7" s="17"/>
-      <c r="S7" s="17"/>
-      <c r="T7" s="17"/>
-      <c r="U7" s="17">
+      <c r="R7" s="22"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22">
         <f t="shared" ref="U7" si="18">HEX2DEC(U6)</f>
         <v>15</v>
       </c>
-      <c r="V7" s="17"/>
-      <c r="W7" s="17"/>
-      <c r="X7" s="17"/>
-      <c r="Y7" s="17">
+      <c r="V7" s="22"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
+      <c r="Y7" s="22">
         <f t="shared" ref="Y7" si="19">HEX2DEC(Y6)</f>
         <v>7</v>
       </c>
-      <c r="Z7" s="17"/>
-      <c r="AA7" s="17"/>
-      <c r="AB7" s="17"/>
-      <c r="AC7" s="17">
+      <c r="Z7" s="22"/>
+      <c r="AA7" s="22"/>
+      <c r="AB7" s="22"/>
+      <c r="AC7" s="22">
         <f t="shared" ref="AC7" si="20">HEX2DEC(AC6)</f>
         <v>15</v>
       </c>
-      <c r="AD7" s="17"/>
-      <c r="AE7" s="17"/>
-      <c r="AF7" s="17"/>
-      <c r="AG7" s="17">
+      <c r="AD7" s="22"/>
+      <c r="AE7" s="22"/>
+      <c r="AF7" s="22"/>
+      <c r="AG7" s="22">
         <f t="shared" ref="AG7" si="21">HEX2DEC(AG6)</f>
         <v>4</v>
       </c>
-      <c r="AH7" s="17"/>
-      <c r="AI7" s="17"/>
-      <c r="AJ7" s="17"/>
-      <c r="AK7" s="16">
+      <c r="AH7" s="22"/>
+      <c r="AI7" s="22"/>
+      <c r="AJ7" s="22"/>
+      <c r="AK7" s="21">
         <f t="shared" ref="AK7" si="22">HEX2DEC(AK6)</f>
         <v>13</v>
       </c>
-      <c r="AL7" s="16"/>
-      <c r="AM7" s="16"/>
-      <c r="AN7" s="16"/>
-      <c r="AO7" s="16">
+      <c r="AL7" s="21"/>
+      <c r="AM7" s="21"/>
+      <c r="AN7" s="21"/>
+      <c r="AO7" s="21">
         <f t="shared" ref="AO7" si="23">HEX2DEC(AO6)</f>
         <v>11</v>
       </c>
-      <c r="AP7" s="16"/>
-      <c r="AQ7" s="16"/>
-      <c r="AR7" s="16"/>
-      <c r="AS7" s="16">
+      <c r="AP7" s="21"/>
+      <c r="AQ7" s="21"/>
+      <c r="AR7" s="21"/>
+      <c r="AS7" s="21">
         <f t="shared" ref="AS7" si="24">HEX2DEC(AS6)</f>
         <v>11</v>
       </c>
-      <c r="AT7" s="16"/>
-      <c r="AU7" s="16"/>
-      <c r="AV7" s="16"/>
-      <c r="AW7" s="16">
+      <c r="AT7" s="21"/>
+      <c r="AU7" s="21"/>
+      <c r="AV7" s="21"/>
+      <c r="AW7" s="21">
         <f t="shared" ref="AW7" si="25">HEX2DEC(AW6)</f>
         <v>8</v>
       </c>
-      <c r="AX7" s="16"/>
-      <c r="AY7" s="16"/>
-      <c r="AZ7" s="16"/>
-      <c r="BA7" s="16">
+      <c r="AX7" s="21"/>
+      <c r="AY7" s="21"/>
+      <c r="AZ7" s="21"/>
+      <c r="BA7" s="21">
         <f>HEX2DEC(BA6)</f>
         <v>6</v>
       </c>
-      <c r="BB7" s="16"/>
-      <c r="BC7" s="16"/>
-      <c r="BD7" s="16"/>
+      <c r="BB7" s="21"/>
+      <c r="BC7" s="21"/>
+      <c r="BD7" s="21"/>
       <c r="BE7" t="s">
         <v>8</v>
       </c>
@@ -1821,13 +1791,13 @@
       <c r="BD9" s="14"/>
     </row>
     <row r="10" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="AK10" s="18" t="str">
+      <c r="AK10" s="23" t="str">
         <f t="shared" ref="AK10" si="26">BIN2HEX(AK9&amp;AL9&amp;AM9&amp;AN9)</f>
         <v>C</v>
       </c>
-      <c r="AL10" s="18"/>
-      <c r="AM10" s="18"/>
-      <c r="AN10" s="18"/>
+      <c r="AL10" s="23"/>
+      <c r="AM10" s="23"/>
+      <c r="AN10" s="23"/>
       <c r="AO10" s="14"/>
       <c r="AP10" s="14"/>
       <c r="AQ10" s="14"/>
@@ -1846,13 +1816,13 @@
       <c r="BD10" s="14"/>
     </row>
     <row r="11" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="AK11" s="18">
+      <c r="AK11" s="23">
         <f t="shared" ref="AK11" si="27">HEX2DEC(AK10)</f>
         <v>12</v>
       </c>
-      <c r="AL11" s="18"/>
-      <c r="AM11" s="18"/>
-      <c r="AN11" s="18"/>
+      <c r="AL11" s="23"/>
+      <c r="AM11" s="23"/>
+      <c r="AN11" s="23"/>
       <c r="AO11" s="14"/>
       <c r="AP11" s="14"/>
       <c r="AQ11" s="14"/>
@@ -2241,207 +2211,207 @@
       </c>
     </row>
     <row r="17" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="str">
+      <c r="A17" s="22" t="str">
         <f t="shared" ref="A17" si="28">BIN2HEX(A16&amp;B16&amp;C16&amp;D16)</f>
         <v>8</v>
       </c>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17" t="str">
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22" t="str">
         <f t="shared" ref="E17" si="29">BIN2HEX(E16&amp;F16&amp;G16&amp;H16)</f>
         <v>0</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17" t="str">
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22" t="str">
         <f t="shared" ref="I17" si="30">BIN2HEX(I16&amp;J16&amp;K16&amp;L16)</f>
         <v>0</v>
       </c>
-      <c r="J17" s="17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17" t="str">
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22" t="str">
         <f t="shared" ref="M17" si="31">BIN2HEX(M16&amp;N16&amp;O16&amp;P16)</f>
         <v>0</v>
       </c>
-      <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
-      <c r="P17" s="17"/>
-      <c r="Q17" s="17" t="str">
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22" t="str">
         <f t="shared" ref="Q17" si="32">BIN2HEX(Q16&amp;R16&amp;S16&amp;T16)</f>
         <v>0</v>
       </c>
-      <c r="R17" s="17"/>
-      <c r="S17" s="17"/>
-      <c r="T17" s="17"/>
-      <c r="U17" s="17" t="str">
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22" t="str">
         <f t="shared" ref="U17" si="33">BIN2HEX(U16&amp;V16&amp;W16&amp;X16)</f>
         <v>F</v>
       </c>
-      <c r="V17" s="17"/>
-      <c r="W17" s="17"/>
-      <c r="X17" s="17"/>
-      <c r="Y17" s="17" t="str">
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22" t="str">
         <f t="shared" ref="Y17" si="34">BIN2HEX(Y16&amp;Z16&amp;AA16&amp;AB16)</f>
         <v>7</v>
       </c>
-      <c r="Z17" s="17"/>
-      <c r="AA17" s="17"/>
-      <c r="AB17" s="17"/>
-      <c r="AC17" s="17" t="str">
+      <c r="Z17" s="22"/>
+      <c r="AA17" s="22"/>
+      <c r="AB17" s="22"/>
+      <c r="AC17" s="22" t="str">
         <f t="shared" ref="AC17" si="35">BIN2HEX(AC16&amp;AD16&amp;AE16&amp;AF16)</f>
         <v>F</v>
       </c>
-      <c r="AD17" s="17"/>
-      <c r="AE17" s="17"/>
-      <c r="AF17" s="17"/>
-      <c r="AG17" s="17" t="str">
+      <c r="AD17" s="22"/>
+      <c r="AE17" s="22"/>
+      <c r="AF17" s="22"/>
+      <c r="AG17" s="22" t="str">
         <f t="shared" ref="AG17" si="36">BIN2HEX(AG16&amp;AH16&amp;AI16&amp;AJ16)</f>
         <v>4</v>
       </c>
-      <c r="AH17" s="17"/>
-      <c r="AI17" s="17"/>
-      <c r="AJ17" s="17"/>
-      <c r="AK17" s="16" t="str">
+      <c r="AH17" s="22"/>
+      <c r="AI17" s="22"/>
+      <c r="AJ17" s="22"/>
+      <c r="AK17" s="21" t="str">
         <f t="shared" ref="AK17" si="37">BIN2HEX(AK16&amp;AL16&amp;AM16&amp;AN16)</f>
         <v>A</v>
       </c>
-      <c r="AL17" s="16"/>
-      <c r="AM17" s="16"/>
-      <c r="AN17" s="16"/>
-      <c r="AO17" s="16" t="str">
+      <c r="AL17" s="21"/>
+      <c r="AM17" s="21"/>
+      <c r="AN17" s="21"/>
+      <c r="AO17" s="21" t="str">
         <f t="shared" ref="AO17" si="38">BIN2HEX(AO16&amp;AP16&amp;AQ16&amp;AR16)</f>
         <v>F</v>
       </c>
-      <c r="AP17" s="16"/>
-      <c r="AQ17" s="16"/>
-      <c r="AR17" s="16"/>
-      <c r="AS17" s="16" t="str">
+      <c r="AP17" s="21"/>
+      <c r="AQ17" s="21"/>
+      <c r="AR17" s="21"/>
+      <c r="AS17" s="21" t="str">
         <f t="shared" ref="AS17" si="39">BIN2HEX(AS16&amp;AT16&amp;AU16&amp;AV16)</f>
         <v>2</v>
       </c>
-      <c r="AT17" s="16"/>
-      <c r="AU17" s="16"/>
-      <c r="AV17" s="16"/>
-      <c r="AW17" s="16" t="str">
+      <c r="AT17" s="21"/>
+      <c r="AU17" s="21"/>
+      <c r="AV17" s="21"/>
+      <c r="AW17" s="21" t="str">
         <f t="shared" ref="AW17" si="40">BIN2HEX(AW16&amp;AX16&amp;AY16&amp;AZ16)</f>
         <v>C</v>
       </c>
-      <c r="AX17" s="16"/>
-      <c r="AY17" s="16"/>
-      <c r="AZ17" s="16"/>
-      <c r="BA17" s="16" t="str">
+      <c r="AX17" s="21"/>
+      <c r="AY17" s="21"/>
+      <c r="AZ17" s="21"/>
+      <c r="BA17" s="21" t="str">
         <f>BIN2HEX(BA16&amp;BB16&amp;BC16&amp;BD16)</f>
         <v>8</v>
       </c>
-      <c r="BB17" s="16"/>
-      <c r="BC17" s="16"/>
-      <c r="BD17" s="16"/>
+      <c r="BB17" s="21"/>
+      <c r="BC17" s="21"/>
+      <c r="BD17" s="21"/>
       <c r="BE17" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+      <c r="A18" s="22">
         <f t="shared" ref="A18" si="41">HEX2DEC(A17)</f>
         <v>8</v>
       </c>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17">
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22">
         <f t="shared" ref="E18" si="42">HEX2DEC(E17)</f>
         <v>0</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17">
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22">
         <f t="shared" ref="I18" si="43">HEX2DEC(I17)</f>
         <v>0</v>
       </c>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-      <c r="M18" s="17">
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="22">
         <f t="shared" ref="M18" si="44">HEX2DEC(M17)</f>
         <v>0</v>
       </c>
-      <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
-      <c r="P18" s="17"/>
-      <c r="Q18" s="17">
+      <c r="N18" s="22"/>
+      <c r="O18" s="22"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22">
         <f t="shared" ref="Q18" si="45">HEX2DEC(Q17)</f>
         <v>0</v>
       </c>
-      <c r="R18" s="17"/>
-      <c r="S18" s="17"/>
-      <c r="T18" s="17"/>
-      <c r="U18" s="17">
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22">
         <f t="shared" ref="U18" si="46">HEX2DEC(U17)</f>
         <v>15</v>
       </c>
-      <c r="V18" s="17"/>
-      <c r="W18" s="17"/>
-      <c r="X18" s="17"/>
-      <c r="Y18" s="17">
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22">
         <f t="shared" ref="Y18" si="47">HEX2DEC(Y17)</f>
         <v>7</v>
       </c>
-      <c r="Z18" s="17"/>
-      <c r="AA18" s="17"/>
-      <c r="AB18" s="17"/>
-      <c r="AC18" s="17">
+      <c r="Z18" s="22"/>
+      <c r="AA18" s="22"/>
+      <c r="AB18" s="22"/>
+      <c r="AC18" s="22">
         <f t="shared" ref="AC18" si="48">HEX2DEC(AC17)</f>
         <v>15</v>
       </c>
-      <c r="AD18" s="17"/>
-      <c r="AE18" s="17"/>
-      <c r="AF18" s="17"/>
-      <c r="AG18" s="17">
+      <c r="AD18" s="22"/>
+      <c r="AE18" s="22"/>
+      <c r="AF18" s="22"/>
+      <c r="AG18" s="22">
         <f t="shared" ref="AG18" si="49">HEX2DEC(AG17)</f>
         <v>4</v>
       </c>
-      <c r="AH18" s="17"/>
-      <c r="AI18" s="17"/>
-      <c r="AJ18" s="17"/>
-      <c r="AK18" s="16">
+      <c r="AH18" s="22"/>
+      <c r="AI18" s="22"/>
+      <c r="AJ18" s="22"/>
+      <c r="AK18" s="21">
         <f t="shared" ref="AK18" si="50">HEX2DEC(AK17)</f>
         <v>10</v>
       </c>
-      <c r="AL18" s="16"/>
-      <c r="AM18" s="16"/>
-      <c r="AN18" s="16"/>
-      <c r="AO18" s="16">
+      <c r="AL18" s="21"/>
+      <c r="AM18" s="21"/>
+      <c r="AN18" s="21"/>
+      <c r="AO18" s="21">
         <f t="shared" ref="AO18" si="51">HEX2DEC(AO17)</f>
         <v>15</v>
       </c>
-      <c r="AP18" s="16"/>
-      <c r="AQ18" s="16"/>
-      <c r="AR18" s="16"/>
-      <c r="AS18" s="16">
+      <c r="AP18" s="21"/>
+      <c r="AQ18" s="21"/>
+      <c r="AR18" s="21"/>
+      <c r="AS18" s="21">
         <f t="shared" ref="AS18" si="52">HEX2DEC(AS17)</f>
         <v>2</v>
       </c>
-      <c r="AT18" s="16"/>
-      <c r="AU18" s="16"/>
-      <c r="AV18" s="16"/>
-      <c r="AW18" s="16">
+      <c r="AT18" s="21"/>
+      <c r="AU18" s="21"/>
+      <c r="AV18" s="21"/>
+      <c r="AW18" s="21">
         <f t="shared" ref="AW18" si="53">HEX2DEC(AW17)</f>
         <v>12</v>
       </c>
-      <c r="AX18" s="16"/>
-      <c r="AY18" s="16"/>
-      <c r="AZ18" s="16"/>
-      <c r="BA18" s="16">
+      <c r="AX18" s="21"/>
+      <c r="AY18" s="21"/>
+      <c r="AZ18" s="21"/>
+      <c r="BA18" s="21">
         <f>HEX2DEC(BA17)</f>
         <v>8</v>
       </c>
-      <c r="BB18" s="16"/>
-      <c r="BC18" s="16"/>
-      <c r="BD18" s="16"/>
+      <c r="BB18" s="21"/>
+      <c r="BC18" s="21"/>
+      <c r="BD18" s="21"/>
       <c r="BE18" t="s">
         <v>8</v>
       </c>
@@ -2641,116 +2611,98 @@
       </c>
     </row>
     <row r="29" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="AK29" s="16" t="str">
+      <c r="AK29" s="21" t="str">
         <f t="shared" ref="AK29" si="54">BIN2HEX(AK28&amp;AL28&amp;AM28&amp;AN28)</f>
         <v>6</v>
       </c>
-      <c r="AL29" s="16"/>
-      <c r="AM29" s="16"/>
-      <c r="AN29" s="16"/>
-      <c r="AO29" s="16" t="str">
+      <c r="AL29" s="21"/>
+      <c r="AM29" s="21"/>
+      <c r="AN29" s="21"/>
+      <c r="AO29" s="21" t="str">
         <f t="shared" ref="AO29" si="55">BIN2HEX(AO28&amp;AP28&amp;AQ28&amp;AR28)</f>
         <v>8</v>
       </c>
-      <c r="AP29" s="16"/>
-      <c r="AQ29" s="16"/>
-      <c r="AR29" s="16"/>
-      <c r="AS29" s="16" t="str">
+      <c r="AP29" s="21"/>
+      <c r="AQ29" s="21"/>
+      <c r="AR29" s="21"/>
+      <c r="AS29" s="21" t="str">
         <f t="shared" ref="AS29" si="56">BIN2HEX(AS28&amp;AT28&amp;AU28&amp;AV28)</f>
         <v>B</v>
       </c>
-      <c r="AT29" s="16"/>
-      <c r="AU29" s="16"/>
-      <c r="AV29" s="16"/>
-      <c r="AW29" s="16" t="str">
+      <c r="AT29" s="21"/>
+      <c r="AU29" s="21"/>
+      <c r="AV29" s="21"/>
+      <c r="AW29" s="21" t="str">
         <f t="shared" ref="AW29" si="57">BIN2HEX(AW28&amp;AX28&amp;AY28&amp;AZ28)</f>
         <v>B</v>
       </c>
-      <c r="AX29" s="16"/>
-      <c r="AY29" s="16"/>
-      <c r="AZ29" s="16"/>
-      <c r="BA29" s="16" t="str">
+      <c r="AX29" s="21"/>
+      <c r="AY29" s="21"/>
+      <c r="AZ29" s="21"/>
+      <c r="BA29" s="21" t="str">
         <f>BIN2HEX(BA28&amp;BB28&amp;BC28&amp;BD28)</f>
         <v>D</v>
       </c>
-      <c r="BB29" s="16"/>
-      <c r="BC29" s="16"/>
-      <c r="BD29" s="16"/>
+      <c r="BB29" s="21"/>
+      <c r="BC29" s="21"/>
+      <c r="BD29" s="21"/>
     </row>
     <row r="30" spans="1:57" x14ac:dyDescent="0.25">
-      <c r="AK30" s="16">
+      <c r="AK30" s="21">
         <f t="shared" ref="AK30" si="58">HEX2DEC(AK29)</f>
         <v>6</v>
       </c>
-      <c r="AL30" s="16"/>
-      <c r="AM30" s="16"/>
-      <c r="AN30" s="16"/>
-      <c r="AO30" s="16">
+      <c r="AL30" s="21"/>
+      <c r="AM30" s="21"/>
+      <c r="AN30" s="21"/>
+      <c r="AO30" s="21">
         <f t="shared" ref="AO30" si="59">HEX2DEC(AO29)</f>
         <v>8</v>
       </c>
-      <c r="AP30" s="16"/>
-      <c r="AQ30" s="16"/>
-      <c r="AR30" s="16"/>
-      <c r="AS30" s="16">
+      <c r="AP30" s="21"/>
+      <c r="AQ30" s="21"/>
+      <c r="AR30" s="21"/>
+      <c r="AS30" s="21">
         <f t="shared" ref="AS30" si="60">HEX2DEC(AS29)</f>
         <v>11</v>
       </c>
-      <c r="AT30" s="16"/>
-      <c r="AU30" s="16"/>
-      <c r="AV30" s="16"/>
-      <c r="AW30" s="16">
+      <c r="AT30" s="21"/>
+      <c r="AU30" s="21"/>
+      <c r="AV30" s="21"/>
+      <c r="AW30" s="21">
         <f t="shared" ref="AW30" si="61">HEX2DEC(AW29)</f>
         <v>11</v>
       </c>
-      <c r="AX30" s="16"/>
-      <c r="AY30" s="16"/>
-      <c r="AZ30" s="16"/>
-      <c r="BA30" s="16">
+      <c r="AX30" s="21"/>
+      <c r="AY30" s="21"/>
+      <c r="AZ30" s="21"/>
+      <c r="BA30" s="21">
         <f>HEX2DEC(BA29)</f>
         <v>13</v>
       </c>
-      <c r="BB30" s="16"/>
-      <c r="BC30" s="16"/>
-      <c r="BD30" s="16"/>
+      <c r="BB30" s="21"/>
+      <c r="BC30" s="21"/>
+      <c r="BD30" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="AO7:AR7"/>
-    <mergeCell ref="AS7:AV7"/>
-    <mergeCell ref="AW7:AZ7"/>
-    <mergeCell ref="BA7:BD7"/>
-    <mergeCell ref="U7:X7"/>
-    <mergeCell ref="Y7:AB7"/>
-    <mergeCell ref="AC7:AF7"/>
-    <mergeCell ref="AG7:AJ7"/>
-    <mergeCell ref="AK7:AN7"/>
-    <mergeCell ref="BA6:BD6"/>
-    <mergeCell ref="U6:X6"/>
-    <mergeCell ref="Y6:AB6"/>
-    <mergeCell ref="AC6:AF6"/>
-    <mergeCell ref="AG6:AJ6"/>
-    <mergeCell ref="AK6:AN6"/>
-    <mergeCell ref="AO6:AR6"/>
-    <mergeCell ref="AS6:AV6"/>
-    <mergeCell ref="AW6:AZ6"/>
-    <mergeCell ref="AK10:AN10"/>
-    <mergeCell ref="AK11:AN11"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="M6:P6"/>
-    <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="M7:P7"/>
-    <mergeCell ref="Q7:T7"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="E17:H17"/>
-    <mergeCell ref="I17:L17"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="Q17:T17"/>
+    <mergeCell ref="AK30:AN30"/>
+    <mergeCell ref="AO30:AR30"/>
+    <mergeCell ref="AS30:AV30"/>
+    <mergeCell ref="AW30:AZ30"/>
+    <mergeCell ref="BA30:BD30"/>
+    <mergeCell ref="BA18:BD18"/>
+    <mergeCell ref="AK29:AN29"/>
+    <mergeCell ref="AO29:AR29"/>
+    <mergeCell ref="AS29:AV29"/>
+    <mergeCell ref="AW29:AZ29"/>
+    <mergeCell ref="BA29:BD29"/>
+    <mergeCell ref="AW18:AZ18"/>
+    <mergeCell ref="AC18:AF18"/>
+    <mergeCell ref="AG18:AJ18"/>
+    <mergeCell ref="AK18:AN18"/>
+    <mergeCell ref="AO18:AR18"/>
+    <mergeCell ref="AS18:AV18"/>
     <mergeCell ref="AS17:AV17"/>
     <mergeCell ref="AW17:AZ17"/>
     <mergeCell ref="BA17:BD17"/>
@@ -2767,23 +2719,41 @@
     <mergeCell ref="AG17:AJ17"/>
     <mergeCell ref="AK17:AN17"/>
     <mergeCell ref="AO17:AR17"/>
-    <mergeCell ref="AC18:AF18"/>
-    <mergeCell ref="AG18:AJ18"/>
-    <mergeCell ref="AK18:AN18"/>
-    <mergeCell ref="AO18:AR18"/>
-    <mergeCell ref="AS18:AV18"/>
-    <mergeCell ref="BA18:BD18"/>
-    <mergeCell ref="AK29:AN29"/>
-    <mergeCell ref="AO29:AR29"/>
-    <mergeCell ref="AS29:AV29"/>
-    <mergeCell ref="AW29:AZ29"/>
-    <mergeCell ref="BA29:BD29"/>
-    <mergeCell ref="AW18:AZ18"/>
-    <mergeCell ref="AK30:AN30"/>
-    <mergeCell ref="AO30:AR30"/>
-    <mergeCell ref="AS30:AV30"/>
-    <mergeCell ref="AW30:AZ30"/>
-    <mergeCell ref="BA30:BD30"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="E17:H17"/>
+    <mergeCell ref="I17:L17"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="Q17:T17"/>
+    <mergeCell ref="AK10:AN10"/>
+    <mergeCell ref="AK11:AN11"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="M6:P6"/>
+    <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="Q7:T7"/>
+    <mergeCell ref="BA6:BD6"/>
+    <mergeCell ref="U6:X6"/>
+    <mergeCell ref="Y6:AB6"/>
+    <mergeCell ref="AC6:AF6"/>
+    <mergeCell ref="AG6:AJ6"/>
+    <mergeCell ref="AK6:AN6"/>
+    <mergeCell ref="AO6:AR6"/>
+    <mergeCell ref="AS6:AV6"/>
+    <mergeCell ref="AW6:AZ6"/>
+    <mergeCell ref="AO7:AR7"/>
+    <mergeCell ref="AS7:AV7"/>
+    <mergeCell ref="AW7:AZ7"/>
+    <mergeCell ref="BA7:BD7"/>
+    <mergeCell ref="U7:X7"/>
+    <mergeCell ref="Y7:AB7"/>
+    <mergeCell ref="AC7:AF7"/>
+    <mergeCell ref="AG7:AJ7"/>
+    <mergeCell ref="AK7:AN7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>